<commit_message>
price declaration handed over to admin
</commit_message>
<xml_diff>
--- a/ADMIN_PRICE.xlsx
+++ b/ADMIN_PRICE.xlsx
@@ -1,54 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhatr\OneDrive\Tkinter\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5E71DB-E15A-4844-92D8-D7DC3CDD9C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>testing 01</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -63,22 +59,84 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -344,21 +402,137 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <cols>
+    <col width="15.7265625" customWidth="1" min="1" max="1"/>
+    <col width="11.81640625" customWidth="1" style="1" min="2" max="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Tiffin</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Chapati</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bhakri</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Bhaji_1</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Bhaji_2</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Varan</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Thepla</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Modak</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Poli</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Half price checkbox included and calculation is adjusted
</commit_message>
<xml_diff>
--- a/ADMIN_PRICE.xlsx
+++ b/ADMIN_PRICE.xlsx
@@ -9,7 +9,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -59,11 +59,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,131 +420,153 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col width="15.7265625" customWidth="1" min="1" max="1"/>
-    <col width="11.81640625" customWidth="1" style="1" min="2" max="2"/>
+    <col width="15.7265625" customWidth="1" style="2" min="1" max="1"/>
+    <col width="11.81640625" customWidth="1" style="3" min="2" max="2"/>
+    <col width="15.08984375" customWidth="1" style="3" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Item</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>Price</t>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>Full Price</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>Half Price</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Tiffin</t>
         </is>
       </c>
       <c r="B2" s="1" t="n">
-        <v>50</v>
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Chapati</t>
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Bhakri</t>
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>Bhaji_1</t>
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>15</v>
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>Bhaji_2</t>
         </is>
       </c>
       <c r="B6" s="1" t="n">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>Varan</t>
         </is>
       </c>
       <c r="B7" s="1" t="n">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>Rice</t>
         </is>
       </c>
       <c r="B8" s="1" t="n">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>Thepla</t>
         </is>
       </c>
       <c r="B9" s="1" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>Modak</t>
         </is>
       </c>
       <c r="B10" s="1" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>Poli</t>
         </is>
       </c>
       <c r="B11" s="1" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="0" algorithmName="SHA-512" sheet="1" objects="1" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="1" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" saltValue="vu8dap2HkEzSaV4t+2fP8Q==" formatRows="1" sort="1" spinCount="100000" hashValue="De7K/20xQSy63BhzQpI2N4UMccFSigahs35p29H836oTV1o5QDvN9Lgq7edUvWJiXWL0Fhgqjqj+mNH1MMlASg=="/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
inserting blank row logic is pending
</commit_message>
<xml_diff>
--- a/ADMIN_PRICE.xlsx
+++ b/ADMIN_PRICE.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" s="1" t="n">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>23</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3">
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -480,7 +480,7 @@
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
@@ -490,10 +490,10 @@
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6">
@@ -503,10 +503,10 @@
         </is>
       </c>
       <c r="B6" s="1" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7">
@@ -516,10 +516,10 @@
         </is>
       </c>
       <c r="B7" s="1" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -529,10 +529,10 @@
         </is>
       </c>
       <c r="B8" s="1" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B9" s="1" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B10" s="1" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B11" s="1" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>